<commit_message>
optimize code and try to use Tableau
</commit_message>
<xml_diff>
--- a/music_channel.xlsx
+++ b/music_channel.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="64">
   <si>
     <t>Channel_name</t>
   </si>
@@ -49,73 +49,51 @@
     <t>Keywords</t>
   </si>
   <si>
+    <t>2CELLOS</t>
+  </si>
+  <si>
+    <t>美波</t>
+  </si>
+  <si>
+    <t>Ado</t>
+  </si>
+  <si>
+    <t>Ayase / YOASOBI</t>
+  </si>
+  <si>
+    <t>星野源</t>
+  </si>
+  <si>
+    <t>kobasolo</t>
+  </si>
+  <si>
+    <t>Ru's Piano Ru味春捲</t>
+  </si>
+  <si>
     <t>Pan Piano</t>
   </si>
   <si>
-    <t>Ayase / YOASOBI</t>
-  </si>
-  <si>
-    <t>2CELLOS</t>
-  </si>
-  <si>
     <t>THE FIRST TAKE</t>
   </si>
   <si>
-    <t>kobasolo</t>
-  </si>
-  <si>
-    <t>Ado</t>
-  </si>
-  <si>
-    <t>星野源</t>
-  </si>
-  <si>
-    <t>美波</t>
-  </si>
-  <si>
-    <t>Ru's Piano Ru味春捲</t>
-  </si>
-  <si>
-    <t>台湾のピアニストです！ 
-アニソンを弾いてます～ 
-良かったら、チャンネル登録お願いします（ベルマークもクリックしましょう！）
-宜しくお願いいたします！
-Welcome to my channel~~
-I make piano covers of  Anime/GAME!
-Please subscribe to my channel and click the bell icon to get new video updates!!
-I am so glad to see new SUB :)
-歡迎來到Pan Piano 小P的音樂工房！
-這邊不定期分享動漫鋼琴演奏！歡迎訂閱與按下旁邊的鈴鐺：）
-官方網站 Offical Website：
-小P的音樂工房http://panpiano.com/ 
-～分享動漫鋼琴演奏與教學～</t>
+    <t>The official home of 2CELLOS - we post our new videos and live concert footage here every few weeks, so keep coming back for the latest 2CELLOS!!</t>
+  </si>
+  <si>
+    <t>【美波 Official Youtube Channel】</t>
+  </si>
+  <si>
+    <t>元気です。</t>
   </si>
   <si>
     <t>ボカロP・Ayase、そしてAyaseがコンポーザーを務めるユニット・YOASOBIのYouTubeチャンネルです。</t>
   </si>
   <si>
-    <t>The official home of 2CELLOS - we post our new videos and live concert footage here every few weeks, so keep coming back for the latest 2CELLOS!!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A microphone and a white studio.
-And 1 rule.
-You’ve got 1 TAKE.
-Perform anything you like.
-Show us everything you’ve got for that 1 moment.
-ONE TAKE ONLY, ONE LIFE ONLY.
-THE FIRST TAKE
-■「THE FIRST TAKE」OFFICIAL SITE: https://www.thefirsttake.jp/
-■「THE FIRST TAKE」 SNS 
-Instagram： https://www.instagram.com/the_firsttake/
-Twitter： https://twitter.com/The_FirstTake
-Tik Tok： https://vt.tiktok.com/ZSJPuQjcF/
-白いスタジオに置かれた、一本のマイク。
-ここでのルールは、ただ一つ。
-一発撮りのパフォーマンスをすること。
-それ以外は、何をしてもいい。
-一度きりのテイクで、何をみせてくれるだろうか。
-一瞬に込められた想いを見逃すな。
-</t>
+    <t>音楽家・俳優・文筆家。
+2010年に1stアルバム『ばかのうた』にてソロデビュー。2016年10月にリリースしたシングル『恋』は、自身も出演したドラマ『逃げるは恥だが役に立つ』の主題歌として社会現象とも呼べる大ヒットを記録した。
+2018年は国民的アニメ映画「映画ドラえもん のび太の宝島」の主題歌、挿入歌を担当。
+そして、2018年12月にリリースしたアルバム『POP VIRUS』は、オリコン週間アルバムランキング、Billboard Japan Hot Albumsにおいて4週連続1位を獲得し、現在も大ヒットを記録中。
+2019年2月から、自身初となる5大ドームツアー“星野源 DOME TOUR 2019『POP VIRUS』”を開催、日本人男性ソロアーティストとして5人目の快挙となる同ツアー全8公演のチケットはすべて即日完売、計33万人を動員した。3月10日の福岡 ヤフオク! ドーム公演を最後に、大盛況ののち全公演を終了した。
+11月からは「Gen Hoshino POP VIRUS World Tour」と題し、ワールド・ツアーの開催も決定。11月23日の上海での公演を皮切りに、ニューヨーク、横浜、台北の4都市で計5公演を行う。</t>
   </si>
   <si>
     <t>毎週金曜19時更新!!音楽プロデューサー、ミュージシャンとして活動するコバソロが贈るエンターテイメントチャンネル!
@@ -127,20 +105,6 @@
 無所属
 I live in Japan and I make music.Everything you see + hear on my page was produced and put together by me.
 Also - I absolutely love hearing feedback from you guys.. so please subscribe and leave a comment!</t>
-  </si>
-  <si>
-    <t>元気です。</t>
-  </si>
-  <si>
-    <t>音楽家・俳優・文筆家。
-2010年に1stアルバム『ばかのうた』にてソロデビュー。2016年10月にリリースしたシングル『恋』は、自身も出演したドラマ『逃げるは恥だが役に立つ』の主題歌として社会現象とも呼べる大ヒットを記録した。
-2018年は国民的アニメ映画「映画ドラえもん のび太の宝島」の主題歌、挿入歌を担当。
-そして、2018年12月にリリースしたアルバム『POP VIRUS』は、オリコン週間アルバムランキング、Billboard Japan Hot Albumsにおいて4週連続1位を獲得し、現在も大ヒットを記録中。
-2019年2月から、自身初となる5大ドームツアー“星野源 DOME TOUR 2019『POP VIRUS』”を開催、日本人男性ソロアーティストとして5人目の快挙となる同ツアー全8公演のチケットはすべて即日完売、計33万人を動員した。3月10日の福岡 ヤフオク! ドーム公演を最後に、大盛況ののち全公演を終了した。
-11月からは「Gen Hoshino POP VIRUS World Tour」と題し、ワールド・ツアーの開催も決定。11月23日の上海での公演を皮切りに、ニューヨーク、横浜、台北の4都市で計5公演を行う。</t>
-  </si>
-  <si>
-    <t>【美波 Official Youtube Channel】</t>
   </si>
   <si>
     <t>I’m RuRu, a piano youtuber from Taiwan.
@@ -168,106 +132,145 @@
 🎹合作洽談/Business：rurupianomusic@gmail.com</t>
   </si>
   <si>
+    <t>台湾のピアニストです！ 
+アニソンを弾いてます～ 
+良かったら、チャンネル登録お願いします（ベルマークもクリックしましょう！）
+宜しくお願いいたします！
+Welcome to my channel~~
+I make piano covers of  Anime/GAME!
+Please subscribe to my channel and click the bell icon to get new video updates!!
+I am so glad to see new SUB :)
+歡迎來到Pan Piano 小P的音樂工房！
+這邊不定期分享動漫鋼琴演奏！歡迎訂閱與按下旁邊的鈴鐺：）
+官方網站 Offical Website：
+小P的音樂工房http://panpiano.com/ 
+～分享動漫鋼琴演奏與教學～</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A microphone and a white studio.
+And 1 rule.
+You’ve got 1 TAKE.
+Perform anything you like.
+Show us everything you’ve got for that 1 moment.
+ONE TAKE ONLY, ONE LIFE ONLY.
+THE FIRST TAKE
+■「THE FIRST TAKE」OFFICIAL SITE: https://www.thefirsttake.jp/
+■「THE FIRST TAKE」 SNS 
+Instagram： https://www.instagram.com/the_firsttake/
+Twitter： https://twitter.com/The_FirstTake
+Tik Tok： https://vt.tiktok.com/ZSJPuQjcF/
+白いスタジオに置かれた、一本のマイク。
+ここでのルールは、ただ一つ。
+一発撮りのパフォーマンスをすること。
+それ以外は、何をしてもいい。
+一度きりのテイクで、何をみせてくれるだろうか。
+一瞬に込められた想いを見逃すな。
+</t>
+  </si>
+  <si>
+    <t>HR</t>
+  </si>
+  <si>
+    <t>JP</t>
+  </si>
+  <si>
     <t>TW</t>
   </si>
   <si>
-    <t>JP</t>
-  </si>
-  <si>
-    <t>HR</t>
+    <t>UUyjuFsbclXyntSRMBAILzbw</t>
+  </si>
+  <si>
+    <t>UU2JzylaIF8qeowc7-5VwwmA</t>
+  </si>
+  <si>
+    <t>UUln9P4Qm3-EAY4aiEPmRwEA</t>
+  </si>
+  <si>
+    <t>UUvpredjG93ifbCP1Y77JyFA</t>
+  </si>
+  <si>
+    <t>UUPKlrgZXnnb89nSeITvTdGA</t>
+  </si>
+  <si>
+    <t>UUDbQblY1XASbgqOXmy6FOFQ</t>
+  </si>
+  <si>
+    <t>UUAYrMNl92jw6cpjdpBP8JyA</t>
   </si>
   <si>
     <t>UUI7ktPB6toqucpkkCiolwLg</t>
   </si>
   <si>
-    <t>UUvpredjG93ifbCP1Y77JyFA</t>
-  </si>
-  <si>
-    <t>UUyjuFsbclXyntSRMBAILzbw</t>
-  </si>
-  <si>
     <t>UU9zY_E8mcAo_Oq772LEZq8Q</t>
   </si>
   <si>
-    <t>UUDbQblY1XASbgqOXmy6FOFQ</t>
-  </si>
-  <si>
-    <t>UUln9P4Qm3-EAY4aiEPmRwEA</t>
-  </si>
-  <si>
-    <t>UUPKlrgZXnnb89nSeITvTdGA</t>
-  </si>
-  <si>
-    <t>UU2JzylaIF8qeowc7-5VwwmA</t>
-  </si>
-  <si>
-    <t>UUAYrMNl92jw6cpjdpBP8JyA</t>
+    <t>['https://en.wikipedia.org/wiki/Independent_music', 'https://en.wikipedia.org/wiki/Pop_music', 'https://en.wikipedia.org/wiki/Music', 'https://en.wikipedia.org/wiki/Classical_music', 'https://en.wikipedia.org/wiki/Rock_music']</t>
+  </si>
+  <si>
+    <t>['https://en.wikipedia.org/wiki/Independent_music', 'https://en.wikipedia.org/wiki/Pop_music', 'https://en.wikipedia.org/wiki/Music', 'https://en.wikipedia.org/wiki/Music_of_Asia', 'https://en.wikipedia.org/wiki/Rock_music']</t>
+  </si>
+  <si>
+    <t>['https://en.wikipedia.org/wiki/Music', 'https://en.wikipedia.org/wiki/Music_of_Asia', 'https://en.wikipedia.org/wiki/Rock_music', 'https://en.wikipedia.org/wiki/Independent_music', 'https://en.wikipedia.org/wiki/Electronic_music', 'https://en.wikipedia.org/wiki/Pop_music']</t>
+  </si>
+  <si>
+    <t>['https://en.wikipedia.org/wiki/Music_of_Asia', 'https://en.wikipedia.org/wiki/Music', 'https://en.wikipedia.org/wiki/Pop_music']</t>
+  </si>
+  <si>
+    <t>['https://en.wikipedia.org/wiki/Music', 'https://en.wikipedia.org/wiki/Music_of_Asia', 'https://en.wikipedia.org/wiki/Pop_music']</t>
+  </si>
+  <si>
+    <t>['https://en.wikipedia.org/wiki/Music', 'https://en.wikipedia.org/wiki/Classical_music', 'https://en.wikipedia.org/wiki/Music_of_Asia']</t>
   </si>
   <si>
     <t>['https://en.wikipedia.org/wiki/Music', 'https://en.wikipedia.org/wiki/Music_of_Asia', 'https://en.wikipedia.org/wiki/Classical_music']</t>
   </si>
   <si>
-    <t>['https://en.wikipedia.org/wiki/Music', 'https://en.wikipedia.org/wiki/Music_of_Asia', 'https://en.wikipedia.org/wiki/Pop_music']</t>
-  </si>
-  <si>
-    <t>['https://en.wikipedia.org/wiki/Rock_music', 'https://en.wikipedia.org/wiki/Pop_music', 'https://en.wikipedia.org/wiki/Music', 'https://en.wikipedia.org/wiki/Independent_music', 'https://en.wikipedia.org/wiki/Classical_music']</t>
-  </si>
-  <si>
-    <t>['https://en.wikipedia.org/wiki/Music', 'https://en.wikipedia.org/wiki/Electronic_music', 'https://en.wikipedia.org/wiki/Rock_music', 'https://en.wikipedia.org/wiki/Independent_music', 'https://en.wikipedia.org/wiki/Pop_music', 'https://en.wikipedia.org/wiki/Music_of_Asia']</t>
-  </si>
-  <si>
-    <t>['https://en.wikipedia.org/wiki/Rock_music', 'https://en.wikipedia.org/wiki/Pop_music', 'https://en.wikipedia.org/wiki/Independent_music', 'https://en.wikipedia.org/wiki/Music_of_Asia', 'https://en.wikipedia.org/wiki/Music']</t>
-  </si>
-  <si>
-    <t>['https://en.wikipedia.org/wiki/Music', 'https://en.wikipedia.org/wiki/Classical_music', 'https://en.wikipedia.org/wiki/Music_of_Asia']</t>
+    <t>https://yt3.ggpht.com/ytc/AMLnZu9V7gXnpIUCJYKKY_KANCGKI-0lrr0VeoRXYVce6A=s800-c-k-c0x00ffffff-no-rj-mo</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/ytc/AMLnZu-a_zfDCmdvUihG0DgQdTY6aPT4lQ5Sst5qnvczgg=s800-c-k-c0x00ffffff-no-rj-mo</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/I3ckNVLPQq04aQklOnRctTEnBjf7pkppVLV7WYe4Nb4g3sge1h-2IlXAvLnRGgrMkMfL4NadPQ=s800-c-k-c0x00ffffff-no-nd-rj</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/ytc/AMLnZu_8o8D8yLIaOLRZMOmVO0fS85nM-VlmWNJHQIJFLQ=s800-c-k-c0x00ffffff-no-rj-mo</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/DLCVX6ArRGaHMe4k4N7Q_QtYiSOwbJ0pHi9zNwegysTq2ozs3G3_CPxImF-2hh0E2SYVGOEc=s800-c-k-c0x00ffffff-no-nd-rj</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/ytc/AMLnZu-9S3og5Ip2zFASnqMWKkjWatBfPT9ELeqUbTSL1A=s800-c-k-c0x00ffffff-no-rj-mo</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/ytc/AMLnZu_-ZUJbCF-LRu259pFVkL4zxoEfNcqq2MNmMccjJw=s800-c-k-c0x00ffffff-no-rj-mo</t>
   </si>
   <si>
     <t>https://yt3.ggpht.com/ytc/AMLnZu-uZODxdm-BCEo0I5izNKjCy33cT6JVQFZ3BkzjzQ=s800-c-k-c0x00ffffff-no-rj</t>
   </si>
   <si>
-    <t>https://yt3.ggpht.com/ytc/AMLnZu_8o8D8yLIaOLRZMOmVO0fS85nM-VlmWNJHQIJFLQ=s800-c-k-c0x00ffffff-no-rj-mo</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/ytc/AMLnZu9V7gXnpIUCJYKKY_KANCGKI-0lrr0VeoRXYVce6A=s800-c-k-c0x00ffffff-no-rj-mo</t>
-  </si>
-  <si>
     <t>https://yt3.ggpht.com/ytc/AMLnZu9H0hC1Gt8ZLT4V9Z5342HDhba7YsApb9sa_0EgvQ=s800-c-k-c0x00ffffff-no-rj</t>
   </si>
   <si>
-    <t>https://yt3.ggpht.com/ytc/AMLnZu-9S3og5Ip2zFASnqMWKkjWatBfPT9ELeqUbTSL1A=s800-c-k-c0x00ffffff-no-rj-mo</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/I3ckNVLPQq04aQklOnRctTEnBjf7pkppVLV7WYe4Nb4g3sge1h-2IlXAvLnRGgrMkMfL4NadPQ=s800-c-k-c0x00ffffff-no-nd-rj</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/DLCVX6ArRGaHMe4k4N7Q_QtYiSOwbJ0pHi9zNwegysTq2ozs3G3_CPxImF-2hh0E2SYVGOEc=s800-c-k-c0x00ffffff-no-nd-rj</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/ytc/AMLnZu-a_zfDCmdvUihG0DgQdTY6aPT4lQ5Sst5qnvczgg=s800-c-k-c0x00ffffff-no-rj-mo</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/ytc/AMLnZu_-ZUJbCF-LRu259pFVkL4zxoEfNcqq2MNmMccjJw=s800-c-k-c0x00ffffff-no-rj-mo</t>
+    <t>2CELLOS Luka Sulic Stjepan Hauser Two Cellos</t>
+  </si>
+  <si>
+    <t>シンガーソングライター</t>
+  </si>
+  <si>
+    <t>アド あぼ ado "アド 歌い手" ADO Ado "Ado TikTok" "アド ティックトック" "Ado 歌い手" 歌い手 "ado 邪魔" エーディーオー エイド うっせぇわ USSEEWA うっせぇわ 会いたくて 踊 レディメイド 夜のピエロ ギラギラ よくばり Ayase</t>
+  </si>
+  <si>
+    <t>星野源 ほしのげん ホシノゲン "Gen Hoshino" "Hoshino Gen" "星野 源"</t>
+  </si>
+  <si>
+    <t>KOBASOLO コバソロ リトルタートルズ 音楽 music インディーズ little turtles live コバ カメ 癒し new 新宿 ストリート タワーレコード ＰＯＰ Ｒ＆Ｂ ＳＯＵＬ ビデオ</t>
+  </si>
+  <si>
+    <t>鋼琴 Ru味春捲 "Ru's Piano" "Ru Piano" Piano ピアノ "Anime Piano" "動漫 鋼琴" Pianist "Piano Cover" RUsPiano 鋼琴女神 "Cosplay Piano" "Cosplay 鋼琴" "ACG ピアノ" ピアノ</t>
   </si>
   <si>
     <t>鋼琴 演奏 ACG 動畫 漫畫 piano ピアノ アニメ 弾いてみた コスプレ パンピアノ "pan piano"</t>
-  </si>
-  <si>
-    <t>2CELLOS Luka Sulic Stjepan Hauser Two Cellos</t>
-  </si>
-  <si>
-    <t>KOBASOLO コバソロ リトルタートルズ 音楽 music インディーズ little turtles live コバ カメ 癒し new 新宿 ストリート タワーレコード ＰＯＰ Ｒ＆Ｂ ＳＯＵＬ ビデオ</t>
-  </si>
-  <si>
-    <t>アド あぼ ado "アド 歌い手" ADO Ado "Ado TikTok" "アド ティックトック" "Ado 歌い手" 歌い手 "ado 邪魔" エーディーオー エイド うっせぇわ USSEEWA うっせぇわ 会いたくて 踊 レディメイド 夜のピエロ ギラギラ よくばり Ayase</t>
-  </si>
-  <si>
-    <t>星野源 ほしのげん ホシノゲン "Gen Hoshino" "Hoshino Gen" "星野 源"</t>
-  </si>
-  <si>
-    <t>シンガーソングライター</t>
-  </si>
-  <si>
-    <t>鋼琴 Ru味春捲 "Ru's Piano" "Ru Piano" Piano ピアノ "Anime Piano" "動漫 鋼琴" Pianist "Piano Cover" RUsPiano 鋼琴女神 "Cosplay Piano" "Cosplay 鋼琴" "ACG ピアノ" ピアノ</t>
   </si>
 </sst>
 </file>
@@ -694,31 +697,31 @@
         <v>20</v>
       </c>
       <c r="D2" s="2">
-        <v>42578</v>
+        <v>40833</v>
       </c>
       <c r="E2" t="s">
         <v>29</v>
       </c>
       <c r="F2">
-        <v>3340000</v>
+        <v>6270000</v>
       </c>
       <c r="G2">
-        <v>518634820</v>
+        <v>1605717035</v>
       </c>
       <c r="H2" t="s">
         <v>32</v>
       </c>
       <c r="I2">
-        <v>538</v>
+        <v>213</v>
       </c>
       <c r="J2" t="s">
         <v>41</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="L2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -732,28 +735,31 @@
         <v>21</v>
       </c>
       <c r="D3" s="2">
-        <v>43420</v>
+        <v>42372</v>
       </c>
       <c r="E3" t="s">
         <v>30</v>
       </c>
       <c r="F3">
-        <v>3960000</v>
+        <v>1300000</v>
       </c>
       <c r="G3">
-        <v>1996303333</v>
+        <v>407899342</v>
       </c>
       <c r="H3" t="s">
         <v>33</v>
       </c>
       <c r="I3">
-        <v>107</v>
+        <v>7</v>
       </c>
       <c r="J3" t="s">
         <v>42</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="L3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -767,31 +773,31 @@
         <v>22</v>
       </c>
       <c r="D4" s="2">
-        <v>40833</v>
+        <v>43330</v>
       </c>
       <c r="E4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F4">
-        <v>6260000</v>
+        <v>3840000</v>
       </c>
       <c r="G4">
-        <v>1604961816</v>
+        <v>1307920219</v>
       </c>
       <c r="H4" t="s">
         <v>34</v>
       </c>
       <c r="I4">
-        <v>213</v>
+        <v>81</v>
       </c>
       <c r="J4" t="s">
         <v>43</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="L4" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -805,28 +811,28 @@
         <v>23</v>
       </c>
       <c r="D5" s="2">
-        <v>43774</v>
+        <v>43420</v>
       </c>
       <c r="E5" t="s">
         <v>30</v>
       </c>
       <c r="F5">
-        <v>6650000</v>
+        <v>3970000</v>
       </c>
       <c r="G5">
-        <v>2317653594</v>
+        <v>1999089792</v>
       </c>
       <c r="H5" t="s">
         <v>35</v>
       </c>
       <c r="I5">
-        <v>413</v>
+        <v>107</v>
       </c>
       <c r="J5" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -840,31 +846,31 @@
         <v>24</v>
       </c>
       <c r="D6" s="2">
-        <v>39629</v>
+        <v>42132</v>
       </c>
       <c r="E6" t="s">
         <v>30</v>
       </c>
       <c r="F6">
-        <v>3000000</v>
+        <v>1460000</v>
       </c>
       <c r="G6">
-        <v>1414086830</v>
+        <v>915916953</v>
       </c>
       <c r="H6" t="s">
         <v>36</v>
       </c>
       <c r="I6">
-        <v>498</v>
+        <v>96</v>
       </c>
       <c r="J6" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="L6" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -878,31 +884,31 @@
         <v>25</v>
       </c>
       <c r="D7" s="2">
-        <v>43330</v>
+        <v>39629</v>
       </c>
       <c r="E7" t="s">
         <v>30</v>
       </c>
       <c r="F7">
-        <v>3810000</v>
+        <v>3000000</v>
       </c>
       <c r="G7">
-        <v>1295340371</v>
+        <v>1414148726</v>
       </c>
       <c r="H7" t="s">
         <v>37</v>
       </c>
       <c r="I7">
-        <v>81</v>
+        <v>498</v>
       </c>
       <c r="J7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="L7" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -916,31 +922,31 @@
         <v>26</v>
       </c>
       <c r="D8" s="2">
-        <v>42132</v>
+        <v>43173</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F8">
-        <v>1460000</v>
+        <v>2250000</v>
       </c>
       <c r="G8">
-        <v>914983335</v>
+        <v>289239844</v>
       </c>
       <c r="H8" t="s">
         <v>38</v>
       </c>
       <c r="I8">
-        <v>96</v>
+        <v>392</v>
       </c>
       <c r="J8" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="L8" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -954,31 +960,31 @@
         <v>27</v>
       </c>
       <c r="D9" s="2">
-        <v>42372</v>
+        <v>42578</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F9">
-        <v>1300000</v>
+        <v>3350000</v>
       </c>
       <c r="G9">
-        <v>407372341</v>
+        <v>519074696</v>
       </c>
       <c r="H9" t="s">
         <v>39</v>
       </c>
       <c r="I9">
-        <v>7</v>
+        <v>539</v>
       </c>
       <c r="J9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -992,31 +998,28 @@
         <v>28</v>
       </c>
       <c r="D10" s="2">
-        <v>43173</v>
+        <v>43774</v>
       </c>
       <c r="E10" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F10">
-        <v>2250000</v>
+        <v>6660000</v>
       </c>
       <c r="G10">
-        <v>288978911</v>
+        <v>2322487900</v>
       </c>
       <c r="H10" t="s">
         <v>40</v>
       </c>
       <c r="I10">
-        <v>391</v>
+        <v>415</v>
       </c>
       <c r="J10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="L10" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Convert tags and topic columns into multiple
</commit_message>
<xml_diff>
--- a/music_channel.xlsx
+++ b/music_channel.xlsx
@@ -49,52 +49,55 @@
     <t>Keywords</t>
   </si>
   <si>
+    <t>THE FIRST TAKE</t>
+  </si>
+  <si>
     <t>Ayase / YOASOBI</t>
   </si>
   <si>
+    <t>kobasolo</t>
+  </si>
+  <si>
+    <t>美波</t>
+  </si>
+  <si>
+    <t>星野源</t>
+  </si>
+  <si>
+    <t>2CELLOS</t>
+  </si>
+  <si>
+    <t>Ru's Piano Ru味春捲</t>
+  </si>
+  <si>
     <t>Ado</t>
   </si>
   <si>
     <t>Pan Piano</t>
   </si>
   <si>
-    <t>kobasolo</t>
-  </si>
-  <si>
-    <t>美波</t>
-  </si>
-  <si>
-    <t>星野源</t>
-  </si>
-  <si>
-    <t>2CELLOS</t>
-  </si>
-  <si>
-    <t>Ru's Piano Ru味春捲</t>
-  </si>
-  <si>
-    <t>THE FIRST TAKE</t>
+    <t xml:space="preserve">A microphone and a white studio.
+And 1 rule.
+You’ve got 1 TAKE.
+Perform anything you like.
+Show us everything you’ve got for that 1 moment.
+ONE TAKE ONLY, ONE LIFE ONLY.
+THE FIRST TAKE
+■「THE FIRST TAKE」OFFICIAL SITE: https://www.thefirsttake.jp/
+■「THE FIRST TAKE」 SNS 
+Instagram： https://www.instagram.com/the_firsttake/
+Twitter： https://twitter.com/The_FirstTake
+Tik Tok： https://vt.tiktok.com/ZSJPuQjcF/
+白いスタジオに置かれた、一本のマイク。
+ここでのルールは、ただ一つ。
+一発撮りのパフォーマンスをすること。
+それ以外は、何をしてもいい。
+一度きりのテイクで、何をみせてくれるだろうか。
+一瞬に込められた想いを見逃すな。
+</t>
   </si>
   <si>
     <t>ボカロP・Ayase、そしてAyaseがコンポーザーを務めるユニット・YOASOBIのYouTubeチャンネルです。</t>
-  </si>
-  <si>
-    <t>元気です。</t>
-  </si>
-  <si>
-    <t>台湾のピアニストです！ 
-アニソンを弾いてます～ 
-良かったら、チャンネル登録お願いします（ベルマークもクリックしましょう！）
-宜しくお願いいたします！
-Welcome to my channel~~
-I make piano covers of  Anime/GAME!
-Please subscribe to my channel and click the bell icon to get new video updates!!
-I am so glad to see new SUB :)
-歡迎來到Pan Piano 小P的音樂工房！
-這邊不定期分享動漫鋼琴演奏！歡迎訂閱與按下旁邊的鈴鐺：）
-官方網站 Offical Website：
-小P的音樂工房http://panpiano.com/ 
-～分享動漫鋼琴演奏與教學～</t>
   </si>
   <si>
     <t>毎週金曜19時更新!!音楽プロデューサー、ミュージシャンとして活動するコバソロが贈るエンターテイメントチャンネル!
@@ -147,124 +150,121 @@
 🎹合作洽談/Business：rurupianomusic@gmail.com</t>
   </si>
   <si>
-    <t xml:space="preserve">A microphone and a white studio.
-And 1 rule.
-You’ve got 1 TAKE.
-Perform anything you like.
-Show us everything you’ve got for that 1 moment.
-ONE TAKE ONLY, ONE LIFE ONLY.
-THE FIRST TAKE
-■「THE FIRST TAKE」OFFICIAL SITE: https://www.thefirsttake.jp/
-■「THE FIRST TAKE」 SNS 
-Instagram： https://www.instagram.com/the_firsttake/
-Twitter： https://twitter.com/The_FirstTake
-Tik Tok： https://vt.tiktok.com/ZSJPuQjcF/
-白いスタジオに置かれた、一本のマイク。
-ここでのルールは、ただ一つ。
-一発撮りのパフォーマンスをすること。
-それ以外は、何をしてもいい。
-一度きりのテイクで、何をみせてくれるだろうか。
-一瞬に込められた想いを見逃すな。
-</t>
+    <t>元気です。</t>
+  </si>
+  <si>
+    <t>台湾のピアニストです！ 
+アニソンを弾いてます～ 
+良かったら、チャンネル登録お願いします（ベルマークもクリックしましょう！）
+宜しくお願いいたします！
+Welcome to my channel~~
+I make piano covers of  Anime/GAME!
+Please subscribe to my channel and click the bell icon to get new video updates!!
+I am so glad to see new SUB :)
+歡迎來到Pan Piano 小P的音樂工房！
+這邊不定期分享動漫鋼琴演奏！歡迎訂閱與按下旁邊的鈴鐺：）
+官方網站 Offical Website：
+小P的音樂工房http://panpiano.com/ 
+～分享動漫鋼琴演奏與教學～</t>
   </si>
   <si>
     <t>JP</t>
   </si>
   <si>
+    <t>HR</t>
+  </si>
+  <si>
     <t>TW</t>
   </si>
   <si>
-    <t>HR</t>
+    <t>UU9zY_E8mcAo_Oq772LEZq8Q</t>
   </si>
   <si>
     <t>UUvpredjG93ifbCP1Y77JyFA</t>
   </si>
   <si>
+    <t>UUDbQblY1XASbgqOXmy6FOFQ</t>
+  </si>
+  <si>
+    <t>UU2JzylaIF8qeowc7-5VwwmA</t>
+  </si>
+  <si>
+    <t>UUPKlrgZXnnb89nSeITvTdGA</t>
+  </si>
+  <si>
+    <t>UUyjuFsbclXyntSRMBAILzbw</t>
+  </si>
+  <si>
+    <t>UUAYrMNl92jw6cpjdpBP8JyA</t>
+  </si>
+  <si>
     <t>UUln9P4Qm3-EAY4aiEPmRwEA</t>
   </si>
   <si>
     <t>UUI7ktPB6toqucpkkCiolwLg</t>
   </si>
   <si>
-    <t>UUDbQblY1XASbgqOXmy6FOFQ</t>
-  </si>
-  <si>
-    <t>UU2JzylaIF8qeowc7-5VwwmA</t>
-  </si>
-  <si>
-    <t>UUPKlrgZXnnb89nSeITvTdGA</t>
-  </si>
-  <si>
-    <t>UUyjuFsbclXyntSRMBAILzbw</t>
-  </si>
-  <si>
-    <t>UUAYrMNl92jw6cpjdpBP8JyA</t>
-  </si>
-  <si>
-    <t>UU9zY_E8mcAo_Oq772LEZq8Q</t>
-  </si>
-  <si>
-    <t>['Music', 'Music_of_Asia', 'Pop_music']</t>
-  </si>
-  <si>
-    <t>['Independent_music', 'Music_of_Asia', 'Music', 'Pop_music', 'Electronic_music', 'Rock_music']</t>
-  </si>
-  <si>
-    <t>['Music', 'Music_of_Asia', 'Classical_music']</t>
-  </si>
-  <si>
-    <t>['Rock_music', 'Independent_music', 'Music', 'Music_of_Asia', 'Pop_music']</t>
-  </si>
-  <si>
-    <t>['Independent_music', 'Classical_music', 'Music', 'Pop_music', 'Rock_music']</t>
+    <t>['Pop_music', 'Music_of_Asia', 'Music']</t>
+  </si>
+  <si>
+    <t>['Pop_music', 'Music', 'Independent_music', 'Rock_music', 'Music_of_Asia']</t>
+  </si>
+  <si>
+    <t>['Classical_music', 'Rock_music', 'Pop_music', 'Music', 'Independent_music']</t>
+  </si>
+  <si>
+    <t>['Classical_music', 'Music_of_Asia', 'Music']</t>
+  </si>
+  <si>
+    <t>['Pop_music', 'Electronic_music', 'Music', 'Music_of_Asia', 'Rock_music', 'Independent_music']</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/ytc/AMLnZu9H0hC1Gt8ZLT4V9Z5342HDhba7YsApb9sa_0EgvQ=s800-c-k-c0x00ffffff-no-rj</t>
   </si>
   <si>
     <t>https://yt3.ggpht.com/ytc/AMLnZu_8o8D8yLIaOLRZMOmVO0fS85nM-VlmWNJHQIJFLQ=s800-c-k-c0x00ffffff-no-rj-mo</t>
   </si>
   <si>
+    <t>https://yt3.ggpht.com/ytc/AMLnZu-9S3og5Ip2zFASnqMWKkjWatBfPT9ELeqUbTSL1A=s800-c-k-c0x00ffffff-no-rj-mo</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/ytc/AMLnZu-a_zfDCmdvUihG0DgQdTY6aPT4lQ5Sst5qnvczgg=s800-c-k-c0x00ffffff-no-rj-mo</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/DLCVX6ArRGaHMe4k4N7Q_QtYiSOwbJ0pHi9zNwegysTq2ozs3G3_CPxImF-2hh0E2SYVGOEc=s800-c-k-c0x00ffffff-no-nd-rj</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/ytc/AMLnZu9V7gXnpIUCJYKKY_KANCGKI-0lrr0VeoRXYVce6A=s800-c-k-c0x00ffffff-no-rj-mo</t>
+  </si>
+  <si>
+    <t>https://yt3.ggpht.com/ytc/AMLnZu_-ZUJbCF-LRu259pFVkL4zxoEfNcqq2MNmMccjJw=s800-c-k-c0x00ffffff-no-rj-mo</t>
+  </si>
+  <si>
     <t>https://yt3.ggpht.com/I3ckNVLPQq04aQklOnRctTEnBjf7pkppVLV7WYe4Nb4g3sge1h-2IlXAvLnRGgrMkMfL4NadPQ=s800-c-k-c0x00ffffff-no-nd-rj</t>
   </si>
   <si>
     <t>https://yt3.ggpht.com/ytc/AMLnZu-uZODxdm-BCEo0I5izNKjCy33cT6JVQFZ3BkzjzQ=s800-c-k-c0x00ffffff-no-rj</t>
   </si>
   <si>
-    <t>https://yt3.ggpht.com/ytc/AMLnZu-9S3og5Ip2zFASnqMWKkjWatBfPT9ELeqUbTSL1A=s800-c-k-c0x00ffffff-no-rj-mo</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/ytc/AMLnZu-a_zfDCmdvUihG0DgQdTY6aPT4lQ5Sst5qnvczgg=s800-c-k-c0x00ffffff-no-rj-mo</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/DLCVX6ArRGaHMe4k4N7Q_QtYiSOwbJ0pHi9zNwegysTq2ozs3G3_CPxImF-2hh0E2SYVGOEc=s800-c-k-c0x00ffffff-no-nd-rj</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/ytc/AMLnZu9V7gXnpIUCJYKKY_KANCGKI-0lrr0VeoRXYVce6A=s800-c-k-c0x00ffffff-no-rj-mo</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/ytc/AMLnZu_-ZUJbCF-LRu259pFVkL4zxoEfNcqq2MNmMccjJw=s800-c-k-c0x00ffffff-no-rj-mo</t>
-  </si>
-  <si>
-    <t>https://yt3.ggpht.com/ytc/AMLnZu9H0hC1Gt8ZLT4V9Z5342HDhba7YsApb9sa_0EgvQ=s800-c-k-c0x00ffffff-no-rj</t>
+    <t>KOBASOLO コバソロ リトルタートルズ 音楽 music インディーズ little turtles live コバ カメ 癒し new 新宿 ストリート タワーレコード ＰＯＰ Ｒ＆Ｂ ＳＯＵＬ ビデオ</t>
+  </si>
+  <si>
+    <t>シンガーソングライター</t>
+  </si>
+  <si>
+    <t>星野源 ほしのげん ホシノゲン "Gen Hoshino" "Hoshino Gen" "星野 源"</t>
+  </si>
+  <si>
+    <t>2CELLOS Luka Sulic Stjepan Hauser Two Cellos</t>
+  </si>
+  <si>
+    <t>鋼琴 Ru味春捲 "Ru's Piano" "Ru Piano" Piano ピアノ "Anime Piano" "動漫 鋼琴" Pianist "Piano Cover" RUsPiano 鋼琴女神 "Cosplay Piano" "Cosplay 鋼琴" "ACG ピアノ" ピアノ</t>
   </si>
   <si>
     <t>アド あぼ ado "アド 歌い手" ADO Ado "Ado TikTok" "アド ティックトック" "Ado 歌い手" 歌い手 "ado 邪魔" エーディーオー エイド うっせぇわ USSEEWA うっせぇわ 会いたくて 踊 レディメイド 夜のピエロ ギラギラ よくばり Ayase</t>
   </si>
   <si>
     <t>鋼琴 演奏 ACG 動畫 漫畫 piano ピアノ アニメ 弾いてみた コスプレ パンピアノ "pan piano"</t>
-  </si>
-  <si>
-    <t>KOBASOLO コバソロ リトルタートルズ 音楽 music インディーズ little turtles live コバ カメ 癒し new 新宿 ストリート タワーレコード ＰＯＰ Ｒ＆Ｂ ＳＯＵＬ ビデオ</t>
-  </si>
-  <si>
-    <t>シンガーソングライター</t>
-  </si>
-  <si>
-    <t>星野源 ほしのげん ホシノゲン "Gen Hoshino" "Hoshino Gen" "星野 源"</t>
-  </si>
-  <si>
-    <t>2CELLOS Luka Sulic Stjepan Hauser Two Cellos</t>
-  </si>
-  <si>
-    <t>鋼琴 Ru味春捲 "Ru's Piano" "Ru Piano" Piano ピアノ "Anime Piano" "動漫 鋼琴" Pianist "Piano Cover" RUsPiano 鋼琴女神 "Cosplay Piano" "Cosplay 鋼琴" "ACG ピアノ" ピアノ</t>
   </si>
 </sst>
 </file>
@@ -691,22 +691,22 @@
         <v>20</v>
       </c>
       <c r="D2" s="2">
-        <v>43420</v>
+        <v>43774</v>
       </c>
       <c r="E2" t="s">
         <v>29</v>
       </c>
       <c r="F2">
-        <v>3980000</v>
+        <v>6740000</v>
       </c>
       <c r="G2">
-        <v>2016671458</v>
+        <v>2372659817</v>
       </c>
       <c r="H2" t="s">
         <v>32</v>
       </c>
       <c r="I2">
-        <v>110</v>
+        <v>422</v>
       </c>
       <c r="J2" t="s">
         <v>41</v>
@@ -726,31 +726,28 @@
         <v>21</v>
       </c>
       <c r="D3" s="2">
-        <v>43330</v>
+        <v>43420</v>
       </c>
       <c r="E3" t="s">
         <v>29</v>
       </c>
       <c r="F3">
-        <v>3960000</v>
+        <v>3980000</v>
       </c>
       <c r="G3">
-        <v>1369159002</v>
+        <v>2024089302</v>
       </c>
       <c r="H3" t="s">
         <v>33</v>
       </c>
       <c r="I3">
-        <v>80</v>
+        <v>111</v>
       </c>
       <c r="J3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="L3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -764,31 +761,31 @@
         <v>22</v>
       </c>
       <c r="D4" s="2">
-        <v>42578</v>
+        <v>39629</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4">
-        <v>3350000</v>
+        <v>3000000</v>
       </c>
       <c r="G4">
-        <v>521228927</v>
+        <v>1418993882</v>
       </c>
       <c r="H4" t="s">
         <v>34</v>
       </c>
       <c r="I4">
-        <v>543</v>
+        <v>499</v>
       </c>
       <c r="J4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>48</v>
       </c>
       <c r="L4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -802,31 +799,31 @@
         <v>23</v>
       </c>
       <c r="D5" s="2">
-        <v>39629</v>
+        <v>42372</v>
       </c>
       <c r="E5" t="s">
         <v>29</v>
       </c>
       <c r="F5">
-        <v>3000000</v>
+        <v>1300000</v>
       </c>
       <c r="G5">
-        <v>1417515169</v>
+        <v>410741180</v>
       </c>
       <c r="H5" t="s">
         <v>35</v>
       </c>
       <c r="I5">
-        <v>499</v>
+        <v>7</v>
       </c>
       <c r="J5" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="K5" s="3" t="s">
         <v>49</v>
       </c>
       <c r="L5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -840,31 +837,31 @@
         <v>24</v>
       </c>
       <c r="D6" s="2">
-        <v>42372</v>
+        <v>42132</v>
       </c>
       <c r="E6" t="s">
         <v>29</v>
       </c>
       <c r="F6">
-        <v>1300000</v>
+        <v>1460000</v>
       </c>
       <c r="G6">
-        <v>409945880</v>
+        <v>921206581</v>
       </c>
       <c r="H6" t="s">
         <v>36</v>
       </c>
       <c r="I6">
-        <v>7</v>
+        <v>96</v>
       </c>
       <c r="J6" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>50</v>
       </c>
       <c r="L6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:12">
@@ -878,31 +875,31 @@
         <v>25</v>
       </c>
       <c r="D7" s="2">
-        <v>42132</v>
+        <v>40833</v>
       </c>
       <c r="E7" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F7">
-        <v>1460000</v>
+        <v>6280000</v>
       </c>
       <c r="G7">
-        <v>919716553</v>
+        <v>1611623530</v>
       </c>
       <c r="H7" t="s">
         <v>37</v>
       </c>
       <c r="I7">
-        <v>96</v>
+        <v>213</v>
       </c>
       <c r="J7" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>51</v>
       </c>
       <c r="L7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:12">
@@ -916,31 +913,31 @@
         <v>26</v>
       </c>
       <c r="D8" s="2">
-        <v>40833</v>
+        <v>43173</v>
       </c>
       <c r="E8" t="s">
         <v>31</v>
       </c>
       <c r="F8">
-        <v>6270000</v>
+        <v>2260000</v>
       </c>
       <c r="G8">
-        <v>1609923110</v>
+        <v>292118685</v>
       </c>
       <c r="H8" t="s">
         <v>38</v>
       </c>
       <c r="I8">
-        <v>213</v>
+        <v>396</v>
       </c>
       <c r="J8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>52</v>
       </c>
       <c r="L8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:12">
@@ -954,31 +951,31 @@
         <v>27</v>
       </c>
       <c r="D9" s="2">
-        <v>43173</v>
+        <v>43330</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F9">
-        <v>2260000</v>
+        <v>4000000</v>
       </c>
       <c r="G9">
-        <v>291322016</v>
+        <v>1392065788</v>
       </c>
       <c r="H9" t="s">
         <v>39</v>
       </c>
       <c r="I9">
-        <v>395</v>
+        <v>80</v>
       </c>
       <c r="J9" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>53</v>
       </c>
       <c r="L9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:12">
@@ -992,28 +989,31 @@
         <v>28</v>
       </c>
       <c r="D10" s="2">
-        <v>43774</v>
+        <v>42578</v>
       </c>
       <c r="E10" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F10">
-        <v>6720000</v>
+        <v>3350000</v>
       </c>
       <c r="G10">
-        <v>2362062682</v>
+        <v>522089417</v>
       </c>
       <c r="H10" t="s">
         <v>40</v>
       </c>
       <c r="I10">
-        <v>420</v>
+        <v>545</v>
       </c>
       <c r="J10" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>54</v>
+      </c>
+      <c r="L10" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>